<commit_message>
Removed unnecessary '=' sign.
</commit_message>
<xml_diff>
--- a/experiments/example.xlsx
+++ b/experiments/example.xlsx
@@ -14,9 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
   <si>
     <t>y</t>
@@ -364,22 +373,19 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <f>1</f>
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <f>2</f>
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <f>3</f>
-        <v>0</v>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <f>B1</f>
@@ -396,18 +402,18 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <f/>
+        <f>(B1 * B2)</f>
         <v>0</v>
       </c>
       <c r="C3">
-        <f>B2</f>
+        <f>(C1 * C2)</f>
         <v>0</v>
       </c>
       <c r="D3">
-        <f>C2</f>
+        <f>(D1 * D2)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Write a df into a specific position of the excel file.
</commit_message>
<xml_diff>
--- a/experiments/example.xlsx
+++ b/experiments/example.xlsx
@@ -1,55 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -68,13 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -362,59 +407,105 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
       </c>
       <c r="B2">
         <f>B1</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="C2">
         <f>C1</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D2">
         <f>D1</f>
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>5</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>z</t>
+        </is>
       </c>
       <c r="B3">
-        <f>(B1 * B2)</f>
-        <v>0</v>
+        <f>(B1 * )</f>
+        <v/>
       </c>
       <c r="C3">
-        <f>(C1 * C2)</f>
-        <v>0</v>
+        <f>(C1 * B2)</f>
+        <v/>
       </c>
       <c r="D3">
-        <f>(D1 * D2)</f>
-        <v>0</v>
+        <f>(D1 * C2)</f>
+        <v/>
+      </c>
+      <c r="E3">
+        <f>E2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>z</t>
+        </is>
+      </c>
+      <c r="C4">
+        <f>(C2 * )</f>
+        <v/>
+      </c>
+      <c r="D4">
+        <f>(D2 * C3)</f>
+        <v/>
+      </c>
+      <c r="E4">
+        <f>(E2 * D3)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed concat reference bug (it was modifying an existing df's column).
</commit_message>
<xml_diff>
--- a/experiments/example.xlsx
+++ b/experiments/example.xlsx
@@ -436,9 +436,10 @@
           <t>z</t>
         </is>
       </c>
-      <c r="D1">
-        <f>(B2 + C2)</f>
-        <v/>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>x_sum</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -457,7 +458,7 @@
         <v/>
       </c>
       <c r="D2">
-        <f>(B3 + C3)</f>
+        <f>SUM(A2:A4)</f>
         <v/>
       </c>
       <c r="E2" t="inlineStr">
@@ -482,7 +483,7 @@
         <v/>
       </c>
       <c r="D3">
-        <f>(B4 + C4)</f>
+        <f>SUM(A2:A4)</f>
         <v/>
       </c>
       <c r="E3">
@@ -506,7 +507,7 @@
         <v/>
       </c>
       <c r="D4">
-        <f>(B5 + C5)</f>
+        <f>SUM(A2:A4)</f>
         <v/>
       </c>
       <c r="E4">
@@ -529,7 +530,7 @@
         <v/>
       </c>
       <c r="D5">
-        <f>(B6 + C6)</f>
+        <f>SUM(A5:A7)</f>
         <v/>
       </c>
     </row>
@@ -548,7 +549,7 @@
         <v/>
       </c>
       <c r="D6">
-        <f>(B7 + C7)</f>
+        <f>SUM(A5:A7)</f>
         <v/>
       </c>
     </row>
@@ -564,6 +565,10 @@
       </c>
       <c r="C7">
         <f>(A7 + B7)</f>
+        <v/>
+      </c>
+      <c r="D7">
+        <f>SUM(A5:A7)</f>
         <v/>
       </c>
     </row>

</xml_diff>